<commit_message>
Sensitive information clean up and readme files added.
</commit_message>
<xml_diff>
--- a/Phenotype/SOURCE_TO_CONCEPT_MAP.xlsx
+++ b/Phenotype/SOURCE_TO_CONCEPT_MAP.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadinai/Documents/GitHub/Genotype:Phenotype-to-OMOP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadinai/Documents/GitHub/ETL-Genotype:Phenotype-to-OMOP/Phenotype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990B0E99-1C12-C945-870E-69CF3EB80681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47EFD9A-A01B-CB45-86B5-F2F35E013EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="500" windowWidth="35080" windowHeight="22180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$26</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="188">
   <si>
     <t>HPO</t>
   </si>
@@ -180,9 +180,6 @@
     <t>invalid_reason</t>
   </si>
   <si>
-    <t>Source_code</t>
-  </si>
-  <si>
     <t>Diminished physical functioning</t>
   </si>
   <si>
@@ -220,6 +217,381 @@
   </si>
   <si>
     <t>Personality changes</t>
+  </si>
+  <si>
+    <t>HP:0001824</t>
+  </si>
+  <si>
+    <t>Weight loss</t>
+  </si>
+  <si>
+    <t>Muscle weakness</t>
+  </si>
+  <si>
+    <t>Night sweats</t>
+  </si>
+  <si>
+    <t>HP:0001324</t>
+  </si>
+  <si>
+    <t>HP:0030166</t>
+  </si>
+  <si>
+    <t>Autoimmunity</t>
+  </si>
+  <si>
+    <t>HP:0002960</t>
+  </si>
+  <si>
+    <t>Cough</t>
+  </si>
+  <si>
+    <t>HP:0012735</t>
+  </si>
+  <si>
+    <t>Dyspnea</t>
+  </si>
+  <si>
+    <t>HP:0002094</t>
+  </si>
+  <si>
+    <t>Chest Pain</t>
+  </si>
+  <si>
+    <t>HP:0100749</t>
+  </si>
+  <si>
+    <t>Hemoptysis</t>
+  </si>
+  <si>
+    <t>Obstruction of the superior vena cava</t>
+  </si>
+  <si>
+    <t>Stridor</t>
+  </si>
+  <si>
+    <t>Hoarse voice</t>
+  </si>
+  <si>
+    <t>Proximal muscle weakness</t>
+  </si>
+  <si>
+    <t>Horner syndrome</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
+    <t>Vertigo</t>
+  </si>
+  <si>
+    <t>Headache</t>
+  </si>
+  <si>
+    <t>Confusion</t>
+  </si>
+  <si>
+    <t>Seizure</t>
+  </si>
+  <si>
+    <t>Anemia</t>
+  </si>
+  <si>
+    <t>Abnormal Blood sodium concentration</t>
+  </si>
+  <si>
+    <t>Leukocytosis</t>
+  </si>
+  <si>
+    <t>Nonproductive cough</t>
+  </si>
+  <si>
+    <t>Malaise</t>
+  </si>
+  <si>
+    <t>Eosinophilia</t>
+  </si>
+  <si>
+    <t>Exertional dyspnea</t>
+  </si>
+  <si>
+    <t>Thrombocytopenia</t>
+  </si>
+  <si>
+    <t>Pharyngalgia</t>
+  </si>
+  <si>
+    <t>Rhinorrhea</t>
+  </si>
+  <si>
+    <t>HP:0002105</t>
+  </si>
+  <si>
+    <t>HP:0031041</t>
+  </si>
+  <si>
+    <t>HP:0010307</t>
+  </si>
+  <si>
+    <t>HP:0001609</t>
+  </si>
+  <si>
+    <t>HP:0003701</t>
+  </si>
+  <si>
+    <t>HP:0002277</t>
+  </si>
+  <si>
+    <t>HP:0012531</t>
+  </si>
+  <si>
+    <t>HP:0002321</t>
+  </si>
+  <si>
+    <t>HP:0002315</t>
+  </si>
+  <si>
+    <t>HP:0001289</t>
+  </si>
+  <si>
+    <t>HP:0001250</t>
+  </si>
+  <si>
+    <t>HP:0001903</t>
+  </si>
+  <si>
+    <t>HP:0010931</t>
+  </si>
+  <si>
+    <t>HP:0001974</t>
+  </si>
+  <si>
+    <t>HP:0031246</t>
+  </si>
+  <si>
+    <t>HP:0033834</t>
+  </si>
+  <si>
+    <t>HP:0001880</t>
+  </si>
+  <si>
+    <t>HP:0002875</t>
+  </si>
+  <si>
+    <t>HP:0001873</t>
+  </si>
+  <si>
+    <t>HP:0033050</t>
+  </si>
+  <si>
+    <t>HP:0031417</t>
+  </si>
+  <si>
+    <t>Palpitations</t>
+  </si>
+  <si>
+    <t>HP:0001962</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>HP:0000739</t>
+  </si>
+  <si>
+    <t>Hyperhidrosis</t>
+  </si>
+  <si>
+    <t>HP:0000975</t>
+  </si>
+  <si>
+    <t>Hand tremor</t>
+  </si>
+  <si>
+    <t>HP:0002378</t>
+  </si>
+  <si>
+    <t>HP:0000711</t>
+  </si>
+  <si>
+    <t>Restlessness</t>
+  </si>
+  <si>
+    <t>Irritability</t>
+  </si>
+  <si>
+    <t>HP:0000737</t>
+  </si>
+  <si>
+    <t>Abnormal eating behavior</t>
+  </si>
+  <si>
+    <t>HP:0100738</t>
+  </si>
+  <si>
+    <t>Heat Intolerance</t>
+  </si>
+  <si>
+    <t>HP:0002046</t>
+  </si>
+  <si>
+    <t>Sleep disturbance</t>
+  </si>
+  <si>
+    <t>HP:0002360</t>
+  </si>
+  <si>
+    <t>Proptosis</t>
+  </si>
+  <si>
+    <t>HP:0000520</t>
+  </si>
+  <si>
+    <t>HP:0046506</t>
+  </si>
+  <si>
+    <t>Pain in head and neck region</t>
+  </si>
+  <si>
+    <t>Abnormality of vision</t>
+  </si>
+  <si>
+    <t>HP:0000504</t>
+  </si>
+  <si>
+    <t>Diplopia</t>
+  </si>
+  <si>
+    <t>Hypogonadism</t>
+  </si>
+  <si>
+    <t>HP:0000135</t>
+  </si>
+  <si>
+    <t>HP:0000651</t>
+  </si>
+  <si>
+    <t>Central adrenal insufficiency</t>
+  </si>
+  <si>
+    <t>HP:0011734</t>
+  </si>
+  <si>
+    <t>Increased body weight</t>
+  </si>
+  <si>
+    <t>HP:0004324</t>
+  </si>
+  <si>
+    <t>HP:0031987</t>
+  </si>
+  <si>
+    <t>Diminished ability to concentrate</t>
+  </si>
+  <si>
+    <t>Constipation</t>
+  </si>
+  <si>
+    <t>Pretibial myxedema</t>
+  </si>
+  <si>
+    <t>Pericardial effusion</t>
+  </si>
+  <si>
+    <t>Dry skin</t>
+  </si>
+  <si>
+    <t>Coldness</t>
+  </si>
+  <si>
+    <t>Bradycardia</t>
+  </si>
+  <si>
+    <t>Hyperlipoproteinemia</t>
+  </si>
+  <si>
+    <t>Hyporeflexia</t>
+  </si>
+  <si>
+    <t>Hypotension</t>
+  </si>
+  <si>
+    <t>Abnormality of the menstrual cycle</t>
+  </si>
+  <si>
+    <t>Gynecomastia</t>
+  </si>
+  <si>
+    <t>Failure to thrive</t>
+  </si>
+  <si>
+    <t>Apathy</t>
+  </si>
+  <si>
+    <t>Thyroid hypoplasia</t>
+  </si>
+  <si>
+    <t>Anti-thyroid peroxidase antibody positivity</t>
+  </si>
+  <si>
+    <t>Regional abnormality of skin</t>
+  </si>
+  <si>
+    <t>Abnormality of temperature regulation</t>
+  </si>
+  <si>
+    <t>HP:0002019</t>
+  </si>
+  <si>
+    <t>HP:0200028</t>
+  </si>
+  <si>
+    <t>HP:0001698</t>
+  </si>
+  <si>
+    <t>HP:0000958</t>
+  </si>
+  <si>
+    <t>HP:0033850</t>
+  </si>
+  <si>
+    <t>HP:0001662</t>
+  </si>
+  <si>
+    <t>HP:0010980</t>
+  </si>
+  <si>
+    <t>HP:0001265</t>
+  </si>
+  <si>
+    <t>HP:0002615</t>
+  </si>
+  <si>
+    <t>HP:0000140</t>
+  </si>
+  <si>
+    <t>HP:0000771</t>
+  </si>
+  <si>
+    <t>HP:0001508</t>
+  </si>
+  <si>
+    <t>HP:0000741</t>
+  </si>
+  <si>
+    <t>HP:0005990</t>
+  </si>
+  <si>
+    <t>HP:0025379</t>
+  </si>
+  <si>
+    <t>HP:0011356</t>
+  </si>
+  <si>
+    <t>HP:0004370</t>
+  </si>
+  <si>
+    <t>source_code</t>
   </si>
 </sst>
 </file>
@@ -227,9 +599,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +620,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +678,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42424C3-CE02-2942-B850-42DA8E7246CC}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -629,7 +1007,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>42</v>
@@ -658,7 +1036,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -666,14 +1044,14 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>31</v>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>31</v>
+      <c r="F2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G2" s="2">
         <v>36526</v>
@@ -685,7 +1063,7 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -693,14 +1071,14 @@
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>51</v>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>51</v>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="2">
         <v>36526</v>
@@ -712,7 +1090,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>
@@ -720,14 +1098,14 @@
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>35</v>
+      <c r="D4" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>35</v>
+      <c r="F4" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G4" s="2">
         <v>36526</v>
@@ -739,7 +1117,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -748,13 +1126,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2">
         <v>36526</v>
@@ -766,7 +1144,7 @@
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -775,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2">
         <v>36526</v>
@@ -793,7 +1171,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="B7" s="5">
         <v>0</v>
@@ -802,13 +1180,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="G7" s="2">
         <v>36526</v>
@@ -820,7 +1198,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -829,13 +1207,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="G8" s="2">
         <v>36526</v>
@@ -847,7 +1225,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -856,13 +1234,13 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="G9" s="2">
         <v>36526</v>
@@ -874,7 +1252,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -883,13 +1261,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="G10" s="2">
         <v>36526</v>
@@ -901,7 +1279,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -910,13 +1288,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2">
         <v>36526</v>
@@ -928,7 +1306,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -937,13 +1315,13 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2">
         <v>36526</v>
@@ -955,7 +1333,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
@@ -964,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="G13" s="2">
         <v>36526</v>
@@ -982,7 +1360,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -991,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="G14" s="2">
         <v>36526</v>
@@ -1009,7 +1387,7 @@
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -1018,13 +1396,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="G15" s="2">
         <v>36526</v>
@@ -1036,7 +1414,7 @@
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
@@ -1045,13 +1423,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G16" s="2">
         <v>36526</v>
@@ -1063,7 +1441,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
@@ -1072,13 +1450,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="G17" s="2">
         <v>36526</v>
@@ -1090,7 +1468,7 @@
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
@@ -1099,13 +1477,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="G18" s="2">
         <v>36526</v>
@@ -1117,7 +1495,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
@@ -1126,13 +1504,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="G19" s="2">
         <v>36526</v>
@@ -1144,7 +1522,7 @@
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
@@ -1153,13 +1531,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G20" s="2">
         <v>36526</v>
@@ -1171,7 +1549,7 @@
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>117</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
@@ -1180,13 +1558,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="G21" s="2">
         <v>36526</v>
@@ -1198,7 +1576,7 @@
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
@@ -1207,13 +1585,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="G22" s="2">
         <v>36526</v>
@@ -1225,7 +1603,7 @@
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5">
         <v>0</v>
@@ -1252,7 +1630,7 @@
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="B24" s="5">
         <v>0</v>
@@ -1261,13 +1639,13 @@
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="G24" s="2">
         <v>36526</v>
@@ -1279,7 +1657,7 @@
     </row>
     <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5">
         <v>0</v>
@@ -1288,13 +1666,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="G25" s="2">
         <v>36526</v>
@@ -1306,7 +1684,7 @@
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="B26" s="5">
         <v>0</v>
@@ -1315,13 +1693,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2">
         <v>36526</v>
@@ -1333,7 +1711,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
       <c r="B27" s="5">
         <v>0</v>
@@ -1342,13 +1720,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="G27" s="2">
         <v>36526</v>
@@ -1360,7 +1738,7 @@
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
@@ -1369,13 +1747,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="G28" s="2">
         <v>36526</v>
@@ -1387,7 +1765,7 @@
     </row>
     <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -1396,13 +1774,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="G29" s="2">
         <v>36526</v>
@@ -1414,7 +1792,7 @@
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B30" s="5">
         <v>0</v>
@@ -1423,13 +1801,13 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="E30" s="5">
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="G30" s="2">
         <v>36526</v>
@@ -1441,7 +1819,7 @@
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="B31" s="5">
         <v>0</v>
@@ -1450,13 +1828,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E31" s="5">
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="G31" s="2">
         <v>36526</v>
@@ -1468,7 +1846,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
@@ -1477,13 +1855,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E32" s="5">
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G32" s="2">
         <v>36526</v>
@@ -1522,7 +1900,7 @@
     </row>
     <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B34" s="5">
         <v>0</v>
@@ -1531,13 +1909,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E34" s="5">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="G34" s="2">
         <v>36526</v>
@@ -1549,7 +1927,7 @@
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5">
         <v>0</v>
@@ -1576,7 +1954,7 @@
     </row>
     <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="B36" s="5">
         <v>0</v>
@@ -1585,13 +1963,13 @@
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E36" s="5">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="G36" s="2">
         <v>36526</v>
@@ -1603,7 +1981,7 @@
     </row>
     <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
@@ -1612,13 +1990,13 @@
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="E37" s="5">
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="G37" s="2">
         <v>36526</v>
@@ -1630,7 +2008,7 @@
     </row>
     <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B38" s="5">
         <v>0</v>
@@ -1657,7 +2035,7 @@
     </row>
     <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -1666,13 +2044,13 @@
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="E39" s="5">
         <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="G39" s="2">
         <v>36526</v>
@@ -1684,7 +2062,7 @@
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="B40" s="5">
         <v>0</v>
@@ -1693,13 +2071,13 @@
         <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E40" s="5">
         <v>0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="G40" s="2">
         <v>36526</v>
@@ -1711,7 +2089,7 @@
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -1720,13 +2098,13 @@
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E41" s="5">
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G41" s="2">
         <v>36526</v>
@@ -1738,7 +2116,7 @@
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -1747,13 +2125,13 @@
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="E42" s="5">
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="G42" s="2">
         <v>36526</v>
@@ -1763,9 +2141,9 @@
       </c>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>10</v>
+        <v>177</v>
       </c>
       <c r="B43" s="5">
         <v>0</v>
@@ -1774,13 +2152,13 @@
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="E43" s="5">
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="G43" s="2">
         <v>36526</v>
@@ -1792,7 +2170,7 @@
     </row>
     <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="B44" s="5">
         <v>0</v>
@@ -1801,13 +2179,13 @@
         <v>0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="E44" s="5">
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="G44" s="2">
         <v>36526</v>
@@ -1819,7 +2197,7 @@
     </row>
     <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B45" s="5">
         <v>0</v>
@@ -1828,13 +2206,13 @@
         <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="E45" s="5">
         <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G45" s="2">
         <v>36526</v>
@@ -1846,7 +2224,7 @@
     </row>
     <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
@@ -1855,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="E46" s="5">
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="G46" s="2">
         <v>36526</v>
@@ -1873,7 +2251,7 @@
     </row>
     <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="B47" s="5">
         <v>0</v>
@@ -1882,13 +2260,13 @@
         <v>0</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="E47" s="5">
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="G47" s="2">
         <v>36526</v>
@@ -1900,7 +2278,7 @@
     </row>
     <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
@@ -1909,13 +2287,13 @@
         <v>0</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E48" s="5">
         <v>0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="G48" s="2">
         <v>36526</v>
@@ -1927,7 +2305,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B49" s="5">
         <v>0</v>
@@ -1936,13 +2314,13 @@
         <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E49" s="5">
         <v>0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G49" s="2">
         <v>36526</v>
@@ -1954,7 +2332,7 @@
     </row>
     <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="B50" s="5">
         <v>0</v>
@@ -1963,13 +2341,13 @@
         <v>0</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="E50" s="5">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G50" s="2">
         <v>36526</v>
@@ -1981,7 +2359,7 @@
     </row>
     <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="B51" s="5">
         <v>0</v>
@@ -1990,13 +2368,13 @@
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="E51" s="5">
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="G51" s="2">
         <v>36526</v>
@@ -2008,7 +2386,7 @@
     </row>
     <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="B52" s="5">
         <v>0</v>
@@ -2017,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="E52" s="5">
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="G52" s="2">
         <v>36526</v>
@@ -2035,7 +2413,7 @@
     </row>
     <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="B53" s="5">
         <v>0</v>
@@ -2044,13 +2422,13 @@
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="E53" s="5">
         <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="G53" s="2">
         <v>36526</v>
@@ -2062,7 +2440,7 @@
     </row>
     <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>16</v>
+        <v>180</v>
       </c>
       <c r="B54" s="5">
         <v>0</v>
@@ -2071,13 +2449,13 @@
         <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="E54" s="5">
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="G54" s="2">
         <v>36526</v>
@@ -2089,7 +2467,7 @@
     </row>
     <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B55" s="5">
         <v>0</v>
@@ -2098,13 +2476,13 @@
         <v>0</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E55" s="5">
         <v>0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="G55" s="2">
         <v>36526</v>
@@ -2116,7 +2494,7 @@
     </row>
     <row r="56" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B56" s="5">
         <v>0</v>
@@ -2125,13 +2503,13 @@
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E56" s="5">
         <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G56" s="2">
         <v>36526</v>
@@ -2143,7 +2521,7 @@
     </row>
     <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B57" s="5">
         <v>0</v>
@@ -2152,13 +2530,13 @@
         <v>0</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E57" s="5">
         <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G57" s="2">
         <v>36526</v>
@@ -2170,7 +2548,7 @@
     </row>
     <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B58" s="5">
         <v>0</v>
@@ -2179,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E58" s="5">
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G58" s="2">
         <v>36526</v>
@@ -2197,7 +2575,7 @@
     </row>
     <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="B59" s="5">
         <v>0</v>
@@ -2206,13 +2584,13 @@
         <v>0</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="E59" s="5">
         <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="G59" s="2">
         <v>36526</v>
@@ -2224,7 +2602,7 @@
     </row>
     <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="B60" s="5">
         <v>0</v>
@@ -2233,13 +2611,13 @@
         <v>0</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="E60" s="5">
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="G60" s="2">
         <v>36526</v>
@@ -2251,7 +2629,7 @@
     </row>
     <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B61" s="5">
         <v>0</v>
@@ -2260,13 +2638,13 @@
         <v>0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="E61" s="5">
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G61" s="2">
         <v>36526</v>
@@ -2278,7 +2656,7 @@
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B62" s="5">
         <v>0</v>
@@ -2287,13 +2665,13 @@
         <v>0</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="E62" s="5">
         <v>0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="G62" s="2">
         <v>36526</v>
@@ -2305,7 +2683,7 @@
     </row>
     <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -2314,13 +2692,13 @@
         <v>0</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E63" s="5">
         <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="G63" s="2">
         <v>36526</v>
@@ -2332,7 +2710,7 @@
     </row>
     <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B64" s="5">
         <v>0</v>
@@ -2341,13 +2719,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E64" s="5">
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G64" s="2">
         <v>36526</v>
@@ -2359,7 +2737,7 @@
     </row>
     <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B65" s="5">
         <v>0</v>
@@ -2368,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E65" s="5">
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G65" s="2">
         <v>36526</v>
@@ -2386,7 +2764,7 @@
     </row>
     <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>22</v>
+        <v>173</v>
       </c>
       <c r="B66" s="5">
         <v>0</v>
@@ -2395,13 +2773,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="E66" s="5">
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="G66" s="2">
         <v>36526</v>
@@ -2413,7 +2791,7 @@
     </row>
     <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="B67" s="5">
         <v>0</v>
@@ -2422,13 +2800,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
       <c r="E67" s="5">
         <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
       <c r="G67" s="2">
         <v>36526</v>
@@ -2440,7 +2818,7 @@
     </row>
     <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B68" s="5">
         <v>0</v>
@@ -2448,14 +2826,14 @@
       <c r="C68" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>41</v>
+      <c r="D68" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="E68" s="5">
         <v>0</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>41</v>
+      <c r="F68" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="G68" s="2">
         <v>36526</v>
@@ -2467,7 +2845,7 @@
     </row>
     <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>25</v>
+        <v>151</v>
       </c>
       <c r="B69" s="5">
         <v>0</v>
@@ -2476,13 +2854,13 @@
         <v>0</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="E69" s="5">
         <v>0</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="G69" s="2">
         <v>36526</v>
@@ -2494,7 +2872,7 @@
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70" s="5">
         <v>0</v>
@@ -2503,13 +2881,13 @@
         <v>0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E70" s="5">
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G70" s="2">
         <v>36526</v>
@@ -2521,7 +2899,7 @@
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B71" s="5">
         <v>0</v>
@@ -2530,13 +2908,13 @@
         <v>0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="E71" s="5">
         <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G71" s="2">
         <v>36526</v>
@@ -2548,7 +2926,7 @@
     </row>
     <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="B72" s="5">
         <v>0</v>
@@ -2557,13 +2935,13 @@
         <v>0</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="E72" s="5">
         <v>0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="G72" s="2">
         <v>36526</v>
@@ -2575,7 +2953,7 @@
     </row>
     <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B73" s="5">
         <v>0</v>
@@ -2584,13 +2962,13 @@
         <v>0</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E73" s="5">
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="G73" s="2">
         <v>36526</v>
@@ -2602,7 +2980,7 @@
     </row>
     <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="B74" s="5">
         <v>0</v>
@@ -2611,13 +2989,13 @@
         <v>0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="E74" s="5">
         <v>0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="G74" s="2">
         <v>36526</v>
@@ -2629,7 +3007,7 @@
     </row>
     <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B75" s="5">
         <v>0</v>
@@ -2638,13 +3016,13 @@
         <v>0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E75" s="5">
         <v>0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="G75" s="2">
         <v>36526</v>
@@ -2654,8 +3032,418 @@
       </c>
       <c r="I75" s="5"/>
     </row>
+    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="5">
+        <v>0</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="5">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G76" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H76" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B77" s="5">
+        <v>0</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G77" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H77" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="5">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G78" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H78" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G79" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H79" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="5">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G80" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H80" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G81" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H81" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E82" s="5">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G82" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H82" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G83" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H83" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G84" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H84" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E85" s="5">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G85" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H85" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B86" s="5">
+        <v>0</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E86" s="5">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G86" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H86" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E87" s="5">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G87" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H87" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B88" s="5">
+        <v>0</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E88" s="5">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G88" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H88" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" s="5">
+        <v>0</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E89" s="5">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G89" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H89" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="5">
+        <v>0</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E90" s="5">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G90" s="2">
+        <v>36526</v>
+      </c>
+      <c r="H90" s="2">
+        <v>73050</v>
+      </c>
+      <c r="I90" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I75" xr:uid="{D42424C3-CE02-2942-B850-42DA8E7246CC}"/>
+  <autoFilter ref="A1:I26" xr:uid="{D42424C3-CE02-2942-B850-42DA8E7246CC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I91">
+      <sortCondition descending="1" ref="D1:D91"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>